<commit_message>
Add Week 05 & Week 06 deliverables
</commit_message>
<xml_diff>
--- a/planning/ProjectPlan_week03_GoldValuePredictor.xlsx
+++ b/planning/ProjectPlan_week03_GoldValuePredictor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d575dc2bf13fc359/Desktop/GoldValue-Predictor/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B807A3C5-0216-488F-8A55-B1A152AA42D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{B807A3C5-0216-488F-8A55-B1A152AA42D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0210417B-1354-449D-AFE4-5362F6D770BA}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D0B153DC-C637-40A9-BCF5-EC09D7DE6F4A}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{D0B153DC-C637-40A9-BCF5-EC09D7DE6F4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>5 days</t>
+  </si>
+  <si>
+    <t>Estimated Cost (RM)</t>
   </si>
 </sst>
 </file>
@@ -487,15 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FBF47D-85E2-4F6E-8C1A-94D18AA8501C}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +520,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -540,8 +546,11 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -561,8 +570,11 @@
         <v>1</v>
       </c>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -582,8 +594,11 @@
         <v>2</v>
       </c>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -603,8 +618,11 @@
         <v>3</v>
       </c>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H5" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -624,8 +642,11 @@
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H6" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -645,8 +666,11 @@
         <v>5</v>
       </c>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -668,8 +692,11 @@
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H8" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -691,8 +718,25 @@
       <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H9" s="2">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2D3109FE-F930-44A9-B190-7543CCE4D0D5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K7">
     <cfRule type="dataBar" priority="2">
       <dataBar>
@@ -707,24 +751,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2D3109FE-F930-44A9-B190-7543CCE4D0D5}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2D3109FE-F930-44A9-B190-7543CCE4D0D5}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{ED311BF5-27A2-49A5-BE4B-B9577C1CC73D}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
@@ -738,19 +781,6 @@
           </x14:cfRule>
           <xm:sqref>K7</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2D3109FE-F930-44A9-B190-7543CCE4D0D5}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C1</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>